<commit_message>
se generaron cambios en la estructura de la pagina, agregar botonera navwegacion y colores
</commit_message>
<xml_diff>
--- a/content/secretaria-ejecutiva/transparencia/art-21-35-guia-de-archivos/guia-de-archivos.xlsx
+++ b/content/secretaria-ejecutiva/transparencia/art-21-35-guia-de-archivos/guia-de-archivos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauragonzalez\Desktop\ESCRITORIO JUNIO 2020\SECRETARÍA EJECUTIVA 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barbaracanales\Documents\TRANSPARENCIA ESTATAL 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BF5AE54-C8FD-4DF5-86C1-46F916D26D4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7925AC42-78F5-4B19-8A93-18DABB064DA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'SECRETARIA TÉCNICA'!$B$2:$J$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">USI!$B$1:$J$25</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="186">
   <si>
     <t>GUIA SIMPLE DE ARCHIVOS DE TRÁMITE DE LA SECRETARÍA EJECUTIVA DEL SISTEMA ANTICORRUPCIÓN DEL ESTADO DE COAHUILA DE ZARAGOZA</t>
   </si>
@@ -596,6 +596,15 @@
   </si>
   <si>
     <t>DIRECCIÓN DE ADMINISTRACIÓN Y FINANZAS</t>
+  </si>
+  <si>
+    <t>844(688 21 78)</t>
+  </si>
+  <si>
+    <t>(844)688 21 78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                             (844)688 21 78</t>
   </si>
 </sst>
 </file>
@@ -1035,63 +1044,99 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1099,6 +1144,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1107,48 +1159,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1160,10 +1175,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1171,12 +1186,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1569,7 +1578,7 @@
   <dimension ref="B1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:J13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1582,17 +1591,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="12"/>
@@ -1606,17 +1615,17 @@
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
@@ -1633,130 +1642,130 @@
       <c r="B6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="45"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="45"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="58"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="45"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="56"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="47"/>
     </row>
     <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="57">
-        <v>8446881546</v>
-      </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="C10" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="60"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="49"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="60"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="49"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="43"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
@@ -1765,15 +1774,15 @@
       <c r="C15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="54"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="51"/>
     </row>
     <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="21" t="s">
@@ -1782,15 +1791,15 @@
       <c r="C16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="41"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="53"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21" t="s">
@@ -1799,15 +1808,15 @@
       <c r="C17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="41"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="53"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="21" t="s">
@@ -1816,15 +1825,15 @@
       <c r="C18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="45"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="55"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="21" t="s">
@@ -1833,15 +1842,15 @@
       <c r="C19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="D19" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="45"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="55"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="21" t="s">
@@ -1850,15 +1859,15 @@
       <c r="C20" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="47"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="57"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="21" t="s">
@@ -1867,15 +1876,15 @@
       <c r="C21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="39"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="59"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="21" t="s">
@@ -1884,15 +1893,15 @@
       <c r="C22" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="45"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="55"/>
     </row>
     <row r="23" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="21" t="s">
@@ -1901,15 +1910,15 @@
       <c r="C23" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="48" t="s">
+      <c r="D23" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="49"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="61"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="21" t="s">
@@ -1918,15 +1927,15 @@
       <c r="C24" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D24" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="39"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="59"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="21" t="s">
@@ -1935,15 +1944,15 @@
       <c r="C25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="39"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="59"/>
     </row>
     <row r="26" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="21" t="s">
@@ -1952,15 +1961,15 @@
       <c r="C26" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="41"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="53"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="21" t="s">
@@ -1969,15 +1978,15 @@
       <c r="C27" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="39"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="59"/>
     </row>
     <row r="28" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="22" t="s">
@@ -1986,43 +1995,43 @@
       <c r="C28" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="43"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D24:J24"/>
+    <mergeCell ref="D25:J25"/>
+    <mergeCell ref="D26:J26"/>
+    <mergeCell ref="D27:J27"/>
+    <mergeCell ref="D28:J28"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="D20:J20"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="D22:J22"/>
+    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="C13:J13"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B4:J4"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="C7:J7"/>
     <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="C13:J13"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="D15:J15"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="D18:J18"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="D20:J20"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="D22:J22"/>
-    <mergeCell ref="D23:J23"/>
-    <mergeCell ref="D24:J24"/>
-    <mergeCell ref="D25:J25"/>
-    <mergeCell ref="D26:J26"/>
-    <mergeCell ref="D27:J27"/>
-    <mergeCell ref="D28:J28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup scale="72" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2037,7 +2046,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection sqref="A1:I28"/>
+      <selection activeCell="B9" sqref="B9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2050,17 +2059,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="86"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="66"/>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
@@ -2074,17 +2083,17 @@
       <c r="I2" s="26"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="74"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="69"/>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
@@ -2101,134 +2110,134 @@
       <c r="A5" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="83"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="71"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="70" t="s">
         <v>176</v>
       </c>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="83"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="71"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="83"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="71"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="81"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="73"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="82">
-        <v>8446881546</v>
-      </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="83"/>
+      <c r="B9" s="70" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="71"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="83"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="71"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="70" t="s">
         <v>177</v>
       </c>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="82"/>
-      <c r="I11" s="83"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="71"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="70" t="s">
         <v>178</v>
       </c>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="83"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="71"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="74"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="69"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
@@ -2237,15 +2246,15 @@
       <c r="B14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="75" t="s">
+      <c r="C14" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="76"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="75"/>
     </row>
     <row r="15" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="33" t="s">
@@ -2254,15 +2263,15 @@
       <c r="B15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="65"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="77"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="33" t="s">
@@ -2271,15 +2280,15 @@
       <c r="B16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="77" t="s">
+      <c r="C16" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
-      <c r="H16" s="77"/>
-      <c r="I16" s="65"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="77"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
@@ -2288,15 +2297,15 @@
       <c r="B17" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="78" t="s">
+      <c r="C17" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="80"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="33" t="s">
@@ -2305,15 +2314,15 @@
       <c r="B18" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C18" s="70" t="s">
+      <c r="C18" s="81" t="s">
         <v>129</v>
       </c>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="71"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="82"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
@@ -2322,15 +2331,15 @@
       <c r="B19" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="70" t="s">
+      <c r="C19" s="81" t="s">
         <v>131</v>
       </c>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="71"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="82"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
@@ -2339,15 +2348,15 @@
       <c r="B20" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="70" t="s">
+      <c r="C20" s="81" t="s">
         <v>133</v>
       </c>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="70"/>
-      <c r="I20" s="71"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="82"/>
     </row>
     <row r="21" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
@@ -2356,15 +2365,15 @@
       <c r="B21" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="C21" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="65"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="77"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="33" t="s">
@@ -2373,15 +2382,15 @@
       <c r="B22" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C22" s="70" t="s">
+      <c r="C22" s="81" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="71"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="82"/>
     </row>
     <row r="23" spans="1:9" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="33" t="s">
@@ -2390,15 +2399,15 @@
       <c r="B23" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C23" s="64" t="s">
+      <c r="C23" s="76" t="s">
         <v>139</v>
       </c>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="65"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="77"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
@@ -2407,15 +2416,15 @@
       <c r="B24" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="66" t="s">
+      <c r="C24" s="83" t="s">
         <v>141</v>
       </c>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="67"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="84"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
@@ -2424,15 +2433,15 @@
       <c r="B25" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="41"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="53"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="33" t="s">
@@ -2441,15 +2450,15 @@
       <c r="B26" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="41"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="53"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="33" t="s">
@@ -2458,15 +2467,15 @@
       <c r="B27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="58" t="s">
         <v>148</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="39"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="59"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="34" t="s">
@@ -2475,44 +2484,44 @@
       <c r="B28" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="85" t="s">
         <v>143</v>
       </c>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="68"/>
-      <c r="I28" s="69"/>
+      <c r="D28" s="85"/>
+      <c r="E28" s="85"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="A13:I13"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="C15:I15"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="C17:I17"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="C19:I19"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C22:I22"/>
     <mergeCell ref="C27:I27"/>
     <mergeCell ref="C23:I23"/>
     <mergeCell ref="C24:I24"/>
     <mergeCell ref="C28:I28"/>
     <mergeCell ref="C25:I25"/>
     <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="C17:I17"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="1.0629921259842521" bottom="1.0629921259842521" header="0.78740157480314965" footer="0.78740157480314965"/>
@@ -2528,7 +2537,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J22"/>
+      <selection activeCell="C9" sqref="C9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2543,17 +2552,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="63"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="40"/>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -2569,17 +2578,17 @@
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="52"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -2598,142 +2607,142 @@
       <c r="B5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="58"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="45"/>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="45"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="93" t="s">
+      <c r="C8" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="94"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="88"/>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="57">
-        <v>8446881546</v>
-      </c>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="58"/>
+      <c r="C9" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="45"/>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="57" t="s">
+      <c r="C12" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="58"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="45"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="52"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="43"/>
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -2743,15 +2752,15 @@
       <c r="C14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="54"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="51"/>
     </row>
     <row r="15" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -2761,15 +2770,15 @@
       <c r="C15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="41"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="53"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -2779,15 +2788,15 @@
       <c r="C16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="41"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="53"/>
     </row>
     <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -2815,15 +2824,15 @@
       <c r="C18" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="91" t="s">
+      <c r="D18" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="91"/>
-      <c r="F18" s="91"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="91"/>
-      <c r="I18" s="91"/>
-      <c r="J18" s="92"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="94"/>
     </row>
     <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -2833,15 +2842,15 @@
       <c r="C19" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="87" t="s">
+      <c r="D19" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="88"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="89"/>
+      <c r="J19" s="90"/>
     </row>
     <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -2851,15 +2860,15 @@
       <c r="C20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="39"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="59"/>
     </row>
     <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
@@ -2869,15 +2878,15 @@
       <c r="C21" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="89" t="s">
+      <c r="D21" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="89"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="89"/>
-      <c r="H21" s="89"/>
-      <c r="I21" s="89"/>
-      <c r="J21" s="90"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="91"/>
+      <c r="I21" s="91"/>
+      <c r="J21" s="92"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
@@ -2887,28 +2896,18 @@
       <c r="C22" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="43"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C12:J12"/>
     <mergeCell ref="D19:J19"/>
     <mergeCell ref="D20:J20"/>
     <mergeCell ref="D21:J21"/>
@@ -2918,6 +2917,16 @@
     <mergeCell ref="D15:J15"/>
     <mergeCell ref="D16:J16"/>
     <mergeCell ref="D18:J18"/>
+    <mergeCell ref="C8:J8"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="1.0629921259842521" bottom="1.0629921259842521" header="0.78740157480314965" footer="0.78740157480314965"/>
@@ -2933,7 +2942,7 @@
   <dimension ref="B1:J22"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J21"/>
+      <selection activeCell="C10" sqref="C10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2946,17 +2955,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="12"/>
@@ -2970,17 +2979,17 @@
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
@@ -2997,134 +3006,134 @@
       <c r="B6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="45"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="45"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="58"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="45"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="93" t="s">
+      <c r="C9" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="88"/>
     </row>
     <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="57">
-        <v>8446881546</v>
-      </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="C10" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="97" t="s">
+      <c r="C12" s="95" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="97"/>
-      <c r="H12" s="97"/>
-      <c r="I12" s="97"/>
-      <c r="J12" s="98"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="95"/>
+      <c r="I12" s="95"/>
+      <c r="J12" s="96"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="97" t="s">
+      <c r="C13" s="95" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="98"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="95"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="95"/>
+      <c r="J13" s="96"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="43"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
@@ -3133,15 +3142,15 @@
       <c r="C15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="54"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="51"/>
     </row>
     <row r="16" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="21" t="s">
@@ -3150,15 +3159,15 @@
       <c r="C16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="41"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="53"/>
     </row>
     <row r="17" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21" t="s">
@@ -3167,15 +3176,15 @@
       <c r="C17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="41"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="53"/>
     </row>
     <row r="18" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="21" t="s">
@@ -3184,15 +3193,15 @@
       <c r="C18" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="41"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="53"/>
     </row>
     <row r="19" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="21" t="s">
@@ -3201,15 +3210,15 @@
       <c r="C19" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="41"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="21" t="s">
@@ -3218,15 +3227,15 @@
       <c r="C20" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="95" t="s">
+      <c r="D20" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="E20" s="95"/>
-      <c r="F20" s="95"/>
-      <c r="G20" s="95"/>
-      <c r="H20" s="95"/>
-      <c r="I20" s="95"/>
-      <c r="J20" s="96"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97"/>
+      <c r="I20" s="97"/>
+      <c r="J20" s="98"/>
     </row>
     <row r="21" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
@@ -3235,31 +3244,21 @@
       <c r="C21" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="43"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="63"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="C13:J13"/>
     <mergeCell ref="D19:J19"/>
     <mergeCell ref="D20:J20"/>
     <mergeCell ref="D21:J21"/>
@@ -3268,6 +3267,16 @@
     <mergeCell ref="D16:J16"/>
     <mergeCell ref="D17:J17"/>
     <mergeCell ref="D18:J18"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="C13:J13"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C8:J8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -3283,7 +3292,7 @@
   <dimension ref="B1:J22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J22"/>
+      <selection activeCell="C10" sqref="C10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3296,17 +3305,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="12"/>
@@ -3320,17 +3329,17 @@
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
@@ -3347,134 +3356,134 @@
       <c r="B6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="45"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="45"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="58"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="45"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="93" t="s">
+      <c r="C9" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="88"/>
     </row>
     <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="57">
-        <v>8446881546</v>
-      </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="C10" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="97" t="s">
+      <c r="C12" s="95" t="s">
         <v>180</v>
       </c>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="97"/>
-      <c r="H12" s="97"/>
-      <c r="I12" s="97"/>
-      <c r="J12" s="98"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="95"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="95"/>
+      <c r="I12" s="95"/>
+      <c r="J12" s="96"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="97" t="s">
+      <c r="C13" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="98"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="95"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="95"/>
+      <c r="J13" s="96"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="43"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
@@ -3483,15 +3492,15 @@
       <c r="C15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="54"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="51"/>
     </row>
     <row r="16" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="21" t="s">
@@ -3500,15 +3509,15 @@
       <c r="C16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="41"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="53"/>
     </row>
     <row r="17" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21" t="s">
@@ -3517,15 +3526,15 @@
       <c r="C17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="49"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="61"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="21" t="s">
@@ -3534,15 +3543,15 @@
       <c r="C18" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="47"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="57"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="21" t="s">
@@ -3551,15 +3560,15 @@
       <c r="C19" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="39"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="59"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="21" t="s">
@@ -3568,15 +3577,15 @@
       <c r="C20" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="39"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="59"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="21" t="s">
@@ -3585,15 +3594,15 @@
       <c r="C21" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="39"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="59"/>
     </row>
     <row r="22" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="22" t="s">
@@ -3602,28 +3611,18 @@
       <c r="C22" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="43"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="C13:J13"/>
     <mergeCell ref="D19:J19"/>
     <mergeCell ref="D20:J20"/>
     <mergeCell ref="D21:J21"/>
@@ -3633,6 +3632,16 @@
     <mergeCell ref="D16:J16"/>
     <mergeCell ref="D17:J17"/>
     <mergeCell ref="D18:J18"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="C13:J13"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C8:J8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -3648,7 +3657,7 @@
   <dimension ref="B1:J25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:J15"/>
+      <selection activeCell="C10" sqref="C10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3661,17 +3670,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="12"/>
@@ -3685,17 +3694,17 @@
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15"/>
@@ -3712,134 +3721,134 @@
       <c r="B6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="45"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="45"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="58"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="45"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="93" t="s">
+      <c r="C9" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="94"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="88"/>
     </row>
     <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="57">
-        <v>8446881546</v>
-      </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="58"/>
+      <c r="C10" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="45"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="57" t="s">
+      <c r="C12" s="44" t="s">
         <v>174</v>
       </c>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="58"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="45"/>
     </row>
     <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="58"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="45"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="43"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
@@ -3848,15 +3857,15 @@
       <c r="C15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="54"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="51"/>
     </row>
     <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="21" t="s">
@@ -3865,15 +3874,15 @@
       <c r="C16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="41"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="53"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21" t="s">
@@ -3890,7 +3899,7 @@
       <c r="G17" s="99"/>
       <c r="H17" s="99"/>
       <c r="I17" s="99"/>
-      <c r="J17" s="41"/>
+      <c r="J17" s="53"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="21" t="s">
@@ -3899,15 +3908,15 @@
       <c r="C18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="39"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="59"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="21" t="s">
@@ -3916,15 +3925,15 @@
       <c r="C19" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="58" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="39"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="59"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="21" t="s">
@@ -3933,15 +3942,15 @@
       <c r="C20" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="39"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="59"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="21" t="s">
@@ -3950,15 +3959,15 @@
       <c r="C21" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="39"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="59"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="21" t="s">
@@ -3967,15 +3976,15 @@
       <c r="C22" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="39"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="59"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="21" t="s">
@@ -3984,15 +3993,15 @@
       <c r="C23" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="39"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="59"/>
     </row>
     <row r="24" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="21" t="s">
@@ -4001,15 +4010,15 @@
       <c r="C24" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="41"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="53"/>
     </row>
     <row r="25" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="22" t="s">
@@ -4018,33 +4027,18 @@
       <c r="C25" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="D25" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="43"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="C13:J13"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="D15:J15"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="D18:J18"/>
     <mergeCell ref="D24:J24"/>
     <mergeCell ref="D25:J25"/>
     <mergeCell ref="D19:J19"/>
@@ -4052,6 +4046,21 @@
     <mergeCell ref="D21:J21"/>
     <mergeCell ref="D22:J22"/>
     <mergeCell ref="D23:J23"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="C13:J13"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C8:J8"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>